<commit_message>
done id check backend
</commit_message>
<xml_diff>
--- a/doc/功能时间计划V1.xlsx
+++ b/doc/功能时间计划V1.xlsx
@@ -228,7 +228,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="170">
   <si>
     <t>文件说明</t>
   </si>
@@ -2593,7 +2593,7 @@
   <dimension ref="A1:K51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2980,6 +2980,12 @@
       </c>
       <c r="G24" s="9">
         <v>2.5</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="I24">
+        <v>8.26</v>
       </c>
     </row>
     <row r="25" spans="1:11" hidden="1">

</xml_diff>

<commit_message>
add model decription doc
</commit_message>
<xml_diff>
--- a/doc/功能时间计划V1.xlsx
+++ b/doc/功能时间计划V1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" showInkAnnotation="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" tabRatio="497"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" tabRatio="497" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="说明" sheetId="1" r:id="rId1"/>
@@ -472,9 +472,6 @@
     <t>保险类别管理</t>
   </si>
   <si>
-    <t>离职原因管理</t>
-  </si>
-  <si>
     <t>缺勤类别管理</t>
   </si>
   <si>
@@ -702,6 +699,9 @@
   </si>
   <si>
     <t>未知</t>
+  </si>
+  <si>
+    <t>离职原因类别管理</t>
   </si>
 </sst>
 </file>
@@ -2121,7 +2121,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A29" sqref="A29:XFD29"/>
     </sheetView>
   </sheetViews>
@@ -2489,19 +2489,19 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:K51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:F52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="11.7109375" style="9" customWidth="1"/>
     <col min="3" max="3" width="27.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="28.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" style="9" customWidth="1"/>
-    <col min="9" max="9" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="0.28515625" style="9" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" style="9" hidden="1" customWidth="1"/>
+    <col min="6" max="7" width="28.140625" style="9" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" style="9" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="45.85546875" customWidth="1"/>
     <col min="11" max="11" width="30.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -2560,7 +2560,7 @@
       <c r="I2" s="12"/>
       <c r="J2" s="12"/>
       <c r="K2" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:11" hidden="1">
@@ -2639,7 +2639,7 @@
         <v>3</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="8" spans="1:11" hidden="1">
@@ -2652,7 +2652,7 @@
       <c r="F8" s="29"/>
       <c r="G8" s="29"/>
       <c r="H8" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="9" spans="1:11" hidden="1">
@@ -2665,7 +2665,7 @@
       <c r="F9" s="29"/>
       <c r="G9" s="29"/>
       <c r="H9" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="10" spans="1:11" hidden="1">
@@ -2678,7 +2678,7 @@
       <c r="F10" s="29"/>
       <c r="G10" s="29"/>
       <c r="H10" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -2689,7 +2689,7 @@
         <v>76</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F11" s="29">
         <v>8</v>
@@ -2705,7 +2705,7 @@
         <v>77</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F12" s="29"/>
       <c r="G12" s="29"/>
@@ -2719,7 +2719,7 @@
         <v>78</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F13" s="29"/>
       <c r="G13" s="29"/>
@@ -2732,7 +2732,7 @@
         <v>79</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F14" s="29"/>
       <c r="G14" s="29"/>
@@ -2745,7 +2745,7 @@
         <v>80</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F15" s="29"/>
       <c r="G15" s="29"/>
@@ -2755,10 +2755,10 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>81</v>
+        <v>157</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F16" s="29"/>
       <c r="G16" s="29"/>
@@ -2768,20 +2768,20 @@
         <v>4.7</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F17" s="29"/>
       <c r="G17" s="29"/>
     </row>
     <row r="18" spans="1:11" hidden="1">
       <c r="B18" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18" s="9" t="s">
         <v>83</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>84</v>
       </c>
       <c r="E18" s="9" t="s">
         <v>41</v>
@@ -2792,10 +2792,10 @@
     </row>
     <row r="19" spans="1:11" hidden="1">
       <c r="B19" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C19" s="9" t="s">
         <v>85</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>86</v>
       </c>
       <c r="E19" s="9" t="s">
         <v>41</v>
@@ -2809,7 +2809,7 @@
         <v>5.2</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E20" s="9" t="s">
         <v>41</v>
@@ -2821,10 +2821,10 @@
     </row>
     <row r="21" spans="1:11" hidden="1">
       <c r="B21" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E21" s="9" t="s">
         <v>41</v>
@@ -2834,10 +2834,10 @@
     </row>
     <row r="22" spans="1:11" s="9" customFormat="1" ht="45" hidden="1" customHeight="1">
       <c r="B22" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C22" s="9" t="s">
         <v>90</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>91</v>
       </c>
       <c r="E22" s="9" t="s">
         <v>36</v>
@@ -2846,15 +2846,15 @@
         <v>8</v>
       </c>
       <c r="J22" s="16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K22" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:11" hidden="1">
       <c r="B23" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>17</v>
@@ -2868,10 +2868,10 @@
     </row>
     <row r="24" spans="1:11" hidden="1">
       <c r="B24" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C24" s="9" t="s">
         <v>93</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>94</v>
       </c>
       <c r="E24" s="9" t="s">
         <v>36</v>
@@ -2891,14 +2891,14 @@
     </row>
     <row r="25" spans="1:11">
       <c r="B25" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D25" s="10"/>
       <c r="E25" s="10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F25" s="10">
         <v>8</v>
@@ -2906,10 +2906,10 @@
     </row>
     <row r="26" spans="1:11" hidden="1">
       <c r="B26" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="C26" s="9" t="s">
         <v>121</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>122</v>
       </c>
       <c r="E26" s="9" t="s">
         <v>36</v>
@@ -2920,23 +2920,23 @@
     </row>
     <row r="27" spans="1:11">
       <c r="B27" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D27" s="10"/>
       <c r="E27" s="10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F27" s="10">
         <v>6</v>
       </c>
       <c r="J27" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K27" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28" spans="1:11" hidden="1">
@@ -2944,21 +2944,21 @@
         <v>5.6</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E28" s="9" t="s">
         <v>41</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="29" spans="1:11" hidden="1">
       <c r="B29" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E29" s="9" t="s">
         <v>41</v>
@@ -2972,10 +2972,10 @@
         <v>61</v>
       </c>
       <c r="B30" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="C30" s="11" t="s">
         <v>96</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>97</v>
       </c>
       <c r="D30" s="11"/>
       <c r="E30" s="11" t="s">
@@ -2987,10 +2987,10 @@
       <c r="G30" s="11"/>
       <c r="H30" s="11"/>
       <c r="J30" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K30" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -2998,10 +2998,10 @@
         <v>6.2</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F31" s="9">
         <v>1</v>
@@ -3012,10 +3012,10 @@
         <v>6.3</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F32" s="9">
         <v>1</v>
@@ -3023,10 +3023,10 @@
     </row>
     <row r="33" spans="1:11" hidden="1">
       <c r="B33" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E33" s="9" t="s">
         <v>36</v>
@@ -3037,10 +3037,10 @@
     </row>
     <row r="34" spans="1:11" hidden="1">
       <c r="B34" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E34" s="9" t="s">
         <v>36</v>
@@ -3054,10 +3054,10 @@
     </row>
     <row r="35" spans="1:11" hidden="1">
       <c r="B35" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="C35" s="9" t="s">
         <v>106</v>
-      </c>
-      <c r="C35" s="9" t="s">
-        <v>107</v>
       </c>
       <c r="E35" s="9" t="s">
         <v>36</v>
@@ -3071,10 +3071,10 @@
     </row>
     <row r="36" spans="1:11" hidden="1">
       <c r="B36" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="C36" s="9" t="s">
         <v>108</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>109</v>
       </c>
       <c r="E36" s="9" t="s">
         <v>36</v>
@@ -3092,7 +3092,7 @@
         <v>7.2</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D37" s="11"/>
       <c r="E37" s="11" t="s">
@@ -3106,13 +3106,13 @@
     </row>
     <row r="38" spans="1:11">
       <c r="B38" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F38" s="9">
         <v>0.5</v>
@@ -3120,13 +3120,13 @@
     </row>
     <row r="39" spans="1:11">
       <c r="B39" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F39" s="9">
         <v>1</v>
@@ -3134,13 +3134,13 @@
     </row>
     <row r="40" spans="1:11">
       <c r="B40" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F40" s="9">
         <v>1.5</v>
@@ -3148,33 +3148,33 @@
     </row>
     <row r="41" spans="1:11">
       <c r="B41" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="C41" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="C41" s="9" t="s">
-        <v>118</v>
-      </c>
       <c r="E41" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F41" s="9">
         <v>4</v>
       </c>
       <c r="J41" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K41" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="42" spans="1:11">
       <c r="B42" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F42" s="9">
         <v>0.5</v>
@@ -3182,13 +3182,13 @@
     </row>
     <row r="43" spans="1:11">
       <c r="B43" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F43" s="9">
         <v>1</v>
@@ -3196,13 +3196,13 @@
     </row>
     <row r="44" spans="1:11">
       <c r="B44" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F44" s="9">
         <v>1.5</v>
@@ -3210,22 +3210,22 @@
     </row>
     <row r="45" spans="1:11">
       <c r="B45" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F45" s="9">
         <v>3</v>
       </c>
       <c r="J45" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K45" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="46" spans="1:11">
@@ -3233,10 +3233,10 @@
         <v>7.5</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F46" s="9">
         <v>3</v>
@@ -3244,13 +3244,13 @@
     </row>
     <row r="47" spans="1:11">
       <c r="B47" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="C47" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="C47" s="9" t="s">
-        <v>139</v>
-      </c>
       <c r="E47" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F47" s="9">
         <v>1</v>
@@ -3258,13 +3258,13 @@
     </row>
     <row r="48" spans="1:11">
       <c r="B48" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="C48" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="C48" s="9" t="s">
-        <v>141</v>
-      </c>
       <c r="E48" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F48" s="9">
         <v>5</v>
@@ -3272,10 +3272,10 @@
     </row>
     <row r="49" spans="2:6" hidden="1">
       <c r="B49" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="C49" s="9" t="s">
         <v>142</v>
-      </c>
-      <c r="C49" s="9" t="s">
-        <v>143</v>
       </c>
       <c r="E49" s="9" t="s">
         <v>41</v>
@@ -3286,13 +3286,13 @@
     </row>
     <row r="50" spans="2:6">
       <c r="B50" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="C50" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="C50" s="9" t="s">
-        <v>145</v>
-      </c>
       <c r="E50" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F50" s="9">
         <v>1</v>
@@ -3300,13 +3300,13 @@
     </row>
     <row r="51" spans="2:6">
       <c r="B51" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="C51" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="C51" s="9" t="s">
-        <v>147</v>
-      </c>
       <c r="E51" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F51" s="9">
         <v>4</v>
@@ -3362,7 +3362,7 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -3372,19 +3372,19 @@
     </row>
     <row r="12" spans="1:6">
       <c r="B12" s="18" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C12" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="E12" s="20" t="s">
         <v>152</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="F12" s="20" t="s">
         <v>154</v>
-      </c>
-      <c r="E12" s="20" t="s">
-        <v>153</v>
-      </c>
-      <c r="F12" s="20" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -3444,7 +3444,7 @@
     </row>
     <row r="16" spans="1:6">
       <c r="B16" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C16" s="22">
         <v>2</v>
@@ -3463,7 +3463,7 @@
     </row>
     <row r="17" spans="2:6">
       <c r="B17" s="21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C17" s="22">
         <v>50.5</v>
@@ -3477,7 +3477,7 @@
     </row>
     <row r="18" spans="2:6">
       <c r="B18" s="21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C18" s="22">
         <v>190</v>

</xml_diff>

<commit_message>
add cal record reasons
</commit_message>
<xml_diff>
--- a/doc/功能时间计划V1.xlsx
+++ b/doc/功能时间计划V1.xlsx
@@ -2490,7 +2490,7 @@
   <dimension ref="A1:K51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2501,7 +2501,7 @@
     <col min="5" max="5" width="14.85546875" style="9" hidden="1" customWidth="1"/>
     <col min="6" max="7" width="28.140625" style="9" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="14.28515625" style="9" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="17.5703125" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="45.85546875" customWidth="1"/>
     <col min="11" max="11" width="30.5703125" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>